<commit_message>
reversed order and logfilepath
</commit_message>
<xml_diff>
--- a/src/CustomAuto/AN.xlsx
+++ b/src/CustomAuto/AN.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103">
   <si>
     <t>分類 \ 編碼原則</t>
   </si>
@@ -93,235 +93,238 @@
     <t>~廠商代號2</t>
   </si>
   <si>
+    <t>原料 - 晶粒細化劑</t>
+  </si>
+  <si>
+    <t>~次分類6</t>
+  </si>
+  <si>
+    <t>原料 - 鋁錠</t>
+  </si>
+  <si>
+    <t>$AL</t>
+  </si>
+  <si>
+    <t>~鋁號(國際編碼四碼)4</t>
+  </si>
+  <si>
+    <t>原料 - 助熔劑</t>
+  </si>
+  <si>
+    <t>$F</t>
+  </si>
+  <si>
+    <t>$L</t>
+  </si>
+  <si>
+    <t>$U</t>
+  </si>
+  <si>
+    <t>$X</t>
+  </si>
+  <si>
+    <t>原料 - 其他</t>
+  </si>
+  <si>
+    <t>~代碼(六碼)6</t>
+  </si>
+  <si>
+    <t>回收料</t>
+  </si>
+  <si>
+    <t>~合金碼6</t>
+  </si>
+  <si>
+    <t>熔煉成品</t>
+  </si>
+  <si>
+    <t>~製程分類2</t>
+  </si>
+  <si>
+    <t>~寸別2</t>
+  </si>
+  <si>
+    <t>~長度(mm)(四碼)4</t>
+  </si>
+  <si>
+    <t>擠型成品、後加工成品</t>
+  </si>
+  <si>
+    <t>~熱處理狀態2</t>
+  </si>
+  <si>
+    <t>~4</t>
+  </si>
+  <si>
+    <t>半成品</t>
+  </si>
+  <si>
+    <t>模具 - 素材</t>
+  </si>
+  <si>
+    <t>形狀</t>
+  </si>
+  <si>
+    <t>~材質區分2</t>
+  </si>
+  <si>
+    <t>加工件分類</t>
+  </si>
+  <si>
+    <t>模具 - 半成品(配件)</t>
+  </si>
+  <si>
+    <t>~類型2</t>
+  </si>
+  <si>
+    <t>~吋別2</t>
+  </si>
+  <si>
+    <t>~材質2</t>
+  </si>
+  <si>
+    <t>~末四碼代碼(自行輸入)4</t>
+  </si>
+  <si>
+    <t>模具 - 半成品(直接擠型-模具&amp;背板)</t>
+  </si>
+  <si>
+    <t>$E</t>
+  </si>
+  <si>
+    <t>類型</t>
+  </si>
+  <si>
+    <t>～厚度4</t>
+  </si>
+  <si>
+    <t>模具 - 半成品(間接擠型-模具&amp;壓餅)</t>
+  </si>
+  <si>
+    <t>$D</t>
+  </si>
+  <si>
+    <t>~內徑尺寸4</t>
+  </si>
+  <si>
+    <t>模具 - 半成品(間接擠型沖心)</t>
+  </si>
+  <si>
+    <t>$M</t>
+  </si>
+  <si>
+    <t>長度</t>
+  </si>
+  <si>
+    <t>~直徑3</t>
+  </si>
+  <si>
+    <t>模具 - 半成品(集團球棒)</t>
+  </si>
+  <si>
+    <t>$A</t>
+  </si>
+  <si>
+    <t>$C</t>
+  </si>
+  <si>
+    <t>直徑</t>
+  </si>
+  <si>
+    <t>~長度3</t>
+  </si>
+  <si>
+    <t>模具 - 半成品(其他)</t>
+  </si>
+  <si>
+    <t>~自行輸入編碼(十一碼)11</t>
+  </si>
+  <si>
+    <t>模具 - 成品(其他)</t>
+  </si>
+  <si>
+    <t>~自行輸入編碼(十碼)10</t>
+  </si>
+  <si>
+    <t>模具 - 成品(抽管)</t>
+  </si>
+  <si>
+    <t>$T</t>
+  </si>
+  <si>
+    <t>~自行輸入編碼(六碼)6</t>
+  </si>
+  <si>
+    <t>模具 - 成品(直接擠型-異型&amp;圓管&amp;板材&amp;配件)</t>
+  </si>
+  <si>
+    <t>~模具設計3</t>
+  </si>
+  <si>
+    <t>~3</t>
+  </si>
+  <si>
+    <t>模具 - 成品(直接擠型-輪圈)</t>
+  </si>
+  <si>
+    <t>$R</t>
+  </si>
+  <si>
+    <t>~自行輸入編碼(三碼)3</t>
+  </si>
+  <si>
+    <t>模具 - 成品(直/間接擠型-專案&amp;圓棒)</t>
+  </si>
+  <si>
+    <t>模具設計</t>
+  </si>
+  <si>
+    <t>~自行輸入編碼(五碼)5</t>
+  </si>
+  <si>
+    <t>模具 - 成品(間接擠型-模具&amp;背板&amp;壓餅-圓&amp;沖心)</t>
+  </si>
+  <si>
+    <t>~尺寸範圍3</t>
+  </si>
+  <si>
+    <t>模具 - 成品(集團球棒)</t>
+  </si>
+  <si>
+    <t>~直徑2</t>
+  </si>
+  <si>
+    <t>~長度2</t>
+  </si>
+  <si>
+    <t>模具 - 成品(間接擠型-壓餅-異型&amp;沖心連接器)</t>
+  </si>
+  <si>
+    <t>模具 - 成品(集團輪圈)</t>
+  </si>
+  <si>
+    <t>~8</t>
+  </si>
+  <si>
+    <t>模具 - 成品(委託)</t>
+  </si>
+  <si>
+    <t>$H</t>
+  </si>
+  <si>
+    <t>$Z</t>
+  </si>
+  <si>
+    <t>~部門別2</t>
+  </si>
+  <si>
+    <t>10CPU</t>
+  </si>
+  <si>
+    <t>穗技廠</t>
+  </si>
+  <si>
     <t>end</t>
-  </si>
-  <si>
-    <t>原料 - 晶粒細化劑</t>
-  </si>
-  <si>
-    <t>~次分類6</t>
-  </si>
-  <si>
-    <t>原料 - 鋁錠</t>
-  </si>
-  <si>
-    <t>$AL</t>
-  </si>
-  <si>
-    <t>~鋁號(國際編碼四碼)4</t>
-  </si>
-  <si>
-    <t>原料 - 助熔劑</t>
-  </si>
-  <si>
-    <t>$F</t>
-  </si>
-  <si>
-    <t>$L</t>
-  </si>
-  <si>
-    <t>$U</t>
-  </si>
-  <si>
-    <t>$X</t>
-  </si>
-  <si>
-    <t>原料 - 其他</t>
-  </si>
-  <si>
-    <t>~代碼(六碼)6</t>
-  </si>
-  <si>
-    <t>回收料</t>
-  </si>
-  <si>
-    <t>~合金碼6</t>
-  </si>
-  <si>
-    <t>熔煉成品</t>
-  </si>
-  <si>
-    <t>~製程分類2</t>
-  </si>
-  <si>
-    <t>~合金別6</t>
-  </si>
-  <si>
-    <t>~寸別2</t>
-  </si>
-  <si>
-    <t>~長度(mm)(四碼)4</t>
-  </si>
-  <si>
-    <t>擠型成品、後加工成品</t>
-  </si>
-  <si>
-    <t>~熱處理狀態2</t>
-  </si>
-  <si>
-    <t>~4</t>
-  </si>
-  <si>
-    <t>半成品</t>
-  </si>
-  <si>
-    <t>模具 - 素材</t>
-  </si>
-  <si>
-    <t>形狀</t>
-  </si>
-  <si>
-    <t>~材質區分2</t>
-  </si>
-  <si>
-    <t>加工件分類</t>
-  </si>
-  <si>
-    <t>模具 - 半成品(配件)</t>
-  </si>
-  <si>
-    <t>~類型2</t>
-  </si>
-  <si>
-    <t>~吋別2</t>
-  </si>
-  <si>
-    <t>~材質2</t>
-  </si>
-  <si>
-    <t>~末四碼代碼(自行輸入)4</t>
-  </si>
-  <si>
-    <t>模具 - 半成品(直接擠型-模具&amp;背板)</t>
-  </si>
-  <si>
-    <t>$E</t>
-  </si>
-  <si>
-    <t>類型</t>
-  </si>
-  <si>
-    <t>～厚度4</t>
-  </si>
-  <si>
-    <t>模具 - 半成品(間接擠型-模具&amp;壓餅)</t>
-  </si>
-  <si>
-    <t>$D</t>
-  </si>
-  <si>
-    <t>~內徑尺寸4</t>
-  </si>
-  <si>
-    <t>模具 - 半成品(間接擠型沖心)</t>
-  </si>
-  <si>
-    <t>$M</t>
-  </si>
-  <si>
-    <t>長度</t>
-  </si>
-  <si>
-    <t>~直徑3</t>
-  </si>
-  <si>
-    <t>模具 - 半成品(集團球棒 )</t>
-  </si>
-  <si>
-    <t>$A</t>
-  </si>
-  <si>
-    <t>$C</t>
-  </si>
-  <si>
-    <t>直徑</t>
-  </si>
-  <si>
-    <t>~長度3</t>
-  </si>
-  <si>
-    <t>模具 - 半成品(其他)</t>
-  </si>
-  <si>
-    <t>~自行輸入編碼(十一碼)11</t>
-  </si>
-  <si>
-    <t>模具 - 成品(其他)</t>
-  </si>
-  <si>
-    <t>~自行輸入編碼(十碼)10</t>
-  </si>
-  <si>
-    <t>模具 - 成品(抽管)</t>
-  </si>
-  <si>
-    <t>$T</t>
-  </si>
-  <si>
-    <t>~自行輸入編碼(六碼)6</t>
-  </si>
-  <si>
-    <t>模具 - 成品(直接擠型-異型&amp;圓管&amp;板材&amp;配件)</t>
-  </si>
-  <si>
-    <t>~模具設計3</t>
-  </si>
-  <si>
-    <t>~3</t>
-  </si>
-  <si>
-    <t>模具 - 成品(直接擠型-輪圈)</t>
-  </si>
-  <si>
-    <t>$R</t>
-  </si>
-  <si>
-    <t>~自行輸入編碼(三碼)3</t>
-  </si>
-  <si>
-    <t>模具 - 成品(直/間接擠型-專案&amp;圓棒)</t>
-  </si>
-  <si>
-    <t>模具設計</t>
-  </si>
-  <si>
-    <t>~自行輸入編碼(五碼)5</t>
-  </si>
-  <si>
-    <t>模具 - 成品(間接擠型-模具&amp;背板&amp;壓餅-圓&amp;沖心)</t>
-  </si>
-  <si>
-    <t>~尺寸範圍3</t>
-  </si>
-  <si>
-    <t>模具 - 成品(集團球棒)</t>
-  </si>
-  <si>
-    <t>~直徑2</t>
-  </si>
-  <si>
-    <t>~長度2</t>
-  </si>
-  <si>
-    <t>模具 - 成品(間接擠型-壓餅-異型&amp;沖心連接器)</t>
-  </si>
-  <si>
-    <t>模具 - 成品(集團輪圈)</t>
-  </si>
-  <si>
-    <t>~8</t>
-  </si>
-  <si>
-    <t>模具 - 成品(委託&amp;維修&amp;維護&amp;氮化)</t>
-  </si>
-  <si>
-    <t>穗技廠</t>
-  </si>
-  <si>
-    <t>$Z</t>
-  </si>
-  <si>
-    <t>~部門別2</t>
   </si>
 </sst>
 </file>
@@ -329,13 +332,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -368,6 +371,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="8.5"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -375,15 +393,100 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -398,100 +501,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -504,9 +515,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -539,19 +549,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -563,31 +717,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -599,127 +729,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -795,6 +805,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -803,16 +824,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -828,15 +849,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -857,27 +869,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -895,7 +905,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -913,134 +923,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1062,9 +1072,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="6" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1085,6 +1092,18 @@
     </xf>
     <xf numFmtId="6" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1417,10 +1436,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E27" sqref="A1:S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="15.5"/>
@@ -1500,7 +1519,7 @@
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
+      <c r="H2" s="6"/>
       <c r="I2" s="5" t="s">
         <v>22</v>
       </c>
@@ -1512,9 +1531,7 @@
         <v>24</v>
       </c>
       <c r="M2" s="6"/>
-      <c r="N2" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="N2" s="6"/>
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
@@ -1523,13 +1540,13 @@
     </row>
     <row r="3" ht="47.25" spans="1:19">
       <c r="A3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -1547,9 +1564,7 @@
         <v>24</v>
       </c>
       <c r="M3" s="6"/>
-      <c r="N3" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
@@ -1558,17 +1573,17 @@
     </row>
     <row r="4" ht="47.25" spans="1:19">
       <c r="A4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -1584,9 +1599,7 @@
         <v>24</v>
       </c>
       <c r="M4" s="6"/>
-      <c r="N4" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
@@ -1595,27 +1608,27 @@
     </row>
     <row r="5" ht="31.75" spans="1:19">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>0</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>0</v>
       </c>
       <c r="I5" s="5" t="s">
@@ -1629,9 +1642,7 @@
         <v>24</v>
       </c>
       <c r="M5" s="6"/>
-      <c r="N5" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
@@ -1640,13 +1651,13 @@
     </row>
     <row r="6" ht="31.75" spans="1:19">
       <c r="A6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="4">
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -1664,9 +1675,7 @@
         <v>24</v>
       </c>
       <c r="M6" s="6"/>
-      <c r="N6" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
@@ -1675,13 +1684,13 @@
     </row>
     <row r="7" ht="31.75" spans="1:19">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="4">
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1699,9 +1708,7 @@
         <v>24</v>
       </c>
       <c r="M7" s="6"/>
-      <c r="N7" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
@@ -1710,20 +1717,20 @@
     </row>
     <row r="8" ht="47.25" spans="1:19">
       <c r="A8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="4">
         <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -1731,36 +1738,34 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M8" s="6"/>
       <c r="N8" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
-      <c r="R8" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="R8" s="6"/>
       <c r="S8" s="6"/>
     </row>
     <row r="9" ht="62.75" spans="1:19">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="4">
         <v>4</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
@@ -1768,36 +1773,34 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M9" s="6"/>
       <c r="N9" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
-      <c r="R9" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="R9" s="6"/>
       <c r="S9" s="6"/>
     </row>
     <row r="10" ht="47.25" spans="1:19">
-      <c r="A10" s="10" t="s">
-        <v>48</v>
+      <c r="A10" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="B10" s="4">
         <v>6</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="5" t="s">
         <v>22</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
@@ -1805,23 +1808,21 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
-      <c r="R10" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="R10" s="6"/>
       <c r="S10" s="6"/>
     </row>
     <row r="11" ht="31.75" spans="1:19">
-      <c r="A11" s="11" t="s">
-        <v>49</v>
+      <c r="A11" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="B11" s="4">
         <v>7</v>
@@ -1829,19 +1830,17 @@
       <c r="C11" s="4">
         <v>2</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
@@ -1855,8 +1854,8 @@
       <c r="S11" s="6"/>
     </row>
     <row r="12" ht="47.25" spans="1:19">
-      <c r="A12" s="11" t="s">
-        <v>53</v>
+      <c r="A12" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="B12" s="4">
         <v>7</v>
@@ -1864,38 +1863,36 @@
       <c r="C12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>54</v>
+      <c r="D12" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="E12" s="6"/>
-      <c r="F12" s="8" t="s">
-        <v>55</v>
+      <c r="F12" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="12" t="s">
-        <v>57</v>
+      <c r="K12" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="N12" s="18"/>
+      <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
     </row>
     <row r="13" ht="78.25" spans="1:19">
-      <c r="A13" s="11" t="s">
-        <v>58</v>
+      <c r="A13" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="B13" s="4">
         <v>7</v>
@@ -1904,39 +1901,37 @@
         <v>22</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K13" s="8" t="s">
-        <v>61</v>
+      <c r="K13" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="N13" s="18"/>
+      <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
     </row>
     <row r="14" ht="78.25" spans="1:19">
-      <c r="A14" s="11" t="s">
-        <v>62</v>
+      <c r="A14" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="B14" s="4">
         <v>7</v>
@@ -1945,39 +1940,37 @@
         <v>22</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="8" t="s">
-        <v>64</v>
+      <c r="K14" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="N14" s="18"/>
+      <c r="O14" s="6"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
     </row>
     <row r="15" ht="62.75" spans="1:19">
-      <c r="A15" s="11" t="s">
-        <v>65</v>
+      <c r="A15" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="B15" s="4">
         <v>7</v>
@@ -1986,41 +1979,39 @@
         <v>22</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>55</v>
+        <v>64</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="L15" s="12" t="s">
-        <v>68</v>
+        <v>65</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>66</v>
       </c>
       <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="N15" s="18"/>
+      <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
     </row>
     <row r="16" ht="47.25" spans="1:19">
-      <c r="A16" s="11" t="s">
-        <v>69</v>
+      <c r="A16" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="B16" s="4">
         <v>7</v>
@@ -2029,10 +2020,10 @@
         <v>22</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F16" s="4">
         <v>0</v>
@@ -2041,31 +2032,29 @@
         <v>0</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="12"/>
+        <v>54</v>
+      </c>
+      <c r="I16" s="11"/>
       <c r="J16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="16" t="s">
-        <v>72</v>
+      <c r="K16" s="19" t="s">
+        <v>70</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M16" s="6"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="N16" s="18"/>
+      <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
     </row>
     <row r="17" ht="62.75" spans="1:19">
-      <c r="A17" s="11" t="s">
-        <v>74</v>
+      <c r="A17" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="B17" s="4">
         <v>7</v>
@@ -2073,8 +2062,8 @@
       <c r="C17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>75</v>
+      <c r="D17" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -2085,24 +2074,22 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="N17" s="18"/>
+      <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
     </row>
     <row r="18" ht="47.25" spans="1:19">
-      <c r="A18" s="11" t="s">
-        <v>76</v>
+      <c r="A18" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="B18" s="4">
         <v>7</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>77</v>
+      <c r="C18" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -2112,10 +2099,8 @@
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="L18" s="18"/>
+      <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
@@ -2124,36 +2109,34 @@
       <c r="S18" s="6"/>
     </row>
     <row r="19" ht="47.25" spans="1:19">
-      <c r="A19" s="11" t="s">
-        <v>78</v>
+      <c r="A19" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="B19" s="4">
         <v>7</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="14">
+        <v>77</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="13">
         <v>0</v>
       </c>
-      <c r="F19" s="14">
+      <c r="F19" s="13">
         <v>0</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="N19" s="17"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="20"/>
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
@@ -2161,35 +2144,33 @@
       <c r="S19" s="6"/>
     </row>
     <row r="20" ht="93.75" spans="1:19">
-      <c r="A20" s="11" t="s">
-        <v>81</v>
+      <c r="A20" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="B20" s="4">
         <v>7</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>60</v>
+      <c r="C20" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K20" s="6"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="L20" s="18"/>
+      <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
@@ -2198,39 +2179,37 @@
       <c r="S20" s="6"/>
     </row>
     <row r="21" ht="62.75" spans="1:19">
-      <c r="A21" s="11" t="s">
-        <v>84</v>
+      <c r="A21" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="B21" s="4">
         <v>7</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>59</v>
+      <c r="C21" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="M21" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="L21" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
@@ -2239,33 +2218,31 @@
       <c r="S21" s="6"/>
     </row>
     <row r="22" ht="78.25" spans="1:19">
-      <c r="A22" s="11" t="s">
-        <v>87</v>
+      <c r="A22" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="B22" s="4">
         <v>7</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>54</v>
+      <c r="C22" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="L22" s="18"/>
+      <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
@@ -2274,35 +2251,33 @@
       <c r="S22" s="6"/>
     </row>
     <row r="23" ht="109.25" spans="1:19">
-      <c r="A23" s="11" t="s">
-        <v>90</v>
+      <c r="A23" s="10" t="s">
+        <v>88</v>
       </c>
       <c r="B23" s="4">
         <v>7</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K23" s="6"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="L23" s="18"/>
+      <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
@@ -2311,17 +2286,17 @@
       <c r="S23" s="6"/>
     </row>
     <row r="24" ht="47.25" spans="1:19">
-      <c r="A24" s="11" t="s">
-        <v>92</v>
+      <c r="A24" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="B24" s="4">
         <v>7</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E24" s="4">
         <v>0</v>
@@ -2336,16 +2311,14 @@
         <v>0</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J24" s="6"/>
       <c r="K24" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="L24" s="15"/>
-      <c r="M24" s="6" t="s">
-        <v>25</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="L24" s="18"/>
+      <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
@@ -2354,33 +2327,31 @@
       <c r="S24" s="6"/>
     </row>
     <row r="25" ht="93.75" spans="1:19">
-      <c r="A25" s="11" t="s">
-        <v>95</v>
+      <c r="A25" s="10" t="s">
+        <v>93</v>
       </c>
       <c r="B25" s="4">
         <v>7</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="L25" s="18"/>
+      <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
@@ -2389,20 +2360,20 @@
       <c r="S25" s="6"/>
     </row>
     <row r="26" ht="47.25" spans="1:19">
-      <c r="A26" s="11" t="s">
-        <v>96</v>
+      <c r="A26" s="10" t="s">
+        <v>94</v>
       </c>
       <c r="B26" s="4">
         <v>7</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -2410,10 +2381,8 @@
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
-      <c r="L26" s="15"/>
-      <c r="M26" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="L26" s="18"/>
+      <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
@@ -2421,18 +2390,18 @@
       <c r="R26" s="6"/>
       <c r="S26" s="6"/>
     </row>
-    <row r="27" ht="78.25" spans="1:19">
-      <c r="A27" s="11" t="s">
-        <v>98</v>
+    <row r="27" ht="31.75" spans="1:19">
+      <c r="A27" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="B27" s="4">
         <v>7</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E27" s="4">
         <v>0</v>
@@ -2441,24 +2410,55 @@
         <v>0</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="L27" s="18"/>
+      <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
       <c r="S27" s="6"/>
+    </row>
+    <row r="28" ht="31.75" spans="1:13">
+      <c r="A28" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="15">
+        <v>7</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" s="15">
+        <v>0</v>
+      </c>
+      <c r="F28" s="15">
+        <v>0</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="H28" s="17"/>
+      <c r="I28" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="L28" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="M28" t="s">
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>